<commit_message>
Use argparse and colors cmd for convert_cc_param, add tool to create the fouling points file
</commit_message>
<xml_diff>
--- a/src/templates/Fouling Points template.xlsx
+++ b/src/templates/Fouling Points template.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Instruction" sheetId="3" r:id="rId2"/>
     <sheet name="Fouling_Point" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -79,9 +79,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +134,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -306,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,9 +320,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -351,18 +354,12 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -390,10 +387,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="174" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -401,6 +398,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,122 +970,122 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="28"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
     </row>
     <row r="21" spans="2:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
+      <c r="B26" s="9"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
+      <c r="B27" s="9"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1090,7 +1093,7 @@
       <c r="C30" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="13">
         <v>40408</v>
       </c>
     </row>
@@ -1098,7 +1101,7 @@
       <c r="C31" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="13"/>
+      <c r="D31" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1153,12 +1156,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1174,7 +1177,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,190 +1189,190 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="30"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="30"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+      <c r="A5" s="30"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="A6" s="30"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="30"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+      <c r="A8" s="30"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="30"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+      <c r="A10" s="30"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+      <c r="A11" s="30"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="30"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="A13" s="30"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+      <c r="A14" s="30"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+      <c r="A15" s="30"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="30"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="30"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
+      <c r="A20" s="30"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+      <c r="A21" s="30"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+      <c r="A22" s="30"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
+      <c r="A23" s="30"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+      <c r="A25" s="30"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+      <c r="A26" s="30"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="30"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="30"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+      <c r="A29" s="30"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+      <c r="A30" s="30"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+      <c r="A31" s="30"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
+      <c r="A32" s="30"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
+      <c r="A33" s="30"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
+      <c r="A34" s="30"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
+      <c r="A35" s="30"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
+      <c r="A36" s="30"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
+      <c r="A37" s="30"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
+      <c r="A38" s="30"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
+      <c r="A39" s="30"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
+      <c r="A40" s="30"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
+      <c r="A41" s="30"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
+      <c r="A42" s="30"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
+      <c r="A43" s="30"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
+      <c r="A44" s="30"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
+      <c r="A45" s="30"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
+      <c r="A46" s="30"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
+      <c r="A47" s="30"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
+      <c r="A48" s="30"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
+      <c r="A49" s="30"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
+      <c r="A50" s="30"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
+      <c r="A51" s="30"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
+      <c r="A52" s="30"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
+      <c r="A53" s="30"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
+      <c r="A54" s="30"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
+      <c r="A55" s="30"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
+      <c r="A56" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1377,5 +1380,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>